<commit_message>
small change to run list for M1 and M2.1
</commit_message>
<xml_diff>
--- a/IO_M1&2.1/RunControl_M1&2.1.xlsx
+++ b/IO_M1&2.1/RunControl_M1&2.1.xlsx
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1422" uniqueCount="380">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1436" uniqueCount="384">
   <si>
     <t>Sheet #</t>
   </si>
@@ -1113,13 +1113,7 @@
     <t>I3F100-1</t>
   </si>
   <si>
-    <t>100% initial Funding; DC 7.5; ir 4.5, SD 4.5%</t>
-  </si>
-  <si>
     <t>I3F100-2</t>
-  </si>
-  <si>
-    <t>100% initial Funding; DC 7.5; ir 6, SD 8.3%</t>
   </si>
   <si>
     <t>I3F100-3</t>
@@ -1128,22 +1122,10 @@
     <t>I3F100-4</t>
   </si>
   <si>
-    <t>100% initial Funding; DC 7.5; ir 9, SD 15.8%</t>
-  </si>
-  <si>
     <t>I3F100-5</t>
   </si>
   <si>
-    <t>100% initial Funding; DC 7.5; ir 10.5, SD 19.5%</t>
-  </si>
-  <si>
     <t>A1F075_soa4</t>
-  </si>
-  <si>
-    <t>75% initial Funding; SOA smoothing: open 15-year cp; 5-year asset smoothing, DR 6.4%, ir 6.4%, sd 12%; Preset MA</t>
-  </si>
-  <si>
-    <t>6.4% / 12%</t>
   </si>
   <si>
     <t>(Individual run)</t>
@@ -1184,7 +1166,37 @@
     <t>75% initial Funding; SOA smoothing: open 15-year cp; 5-year asset smoothing, DR 5.9%, ir 5.9%, sd 12%; Preset MA</t>
   </si>
   <si>
-    <t>5.9% / 12%</t>
+    <t>75% initial Funding; SOA smoothing: open 15-year cp; 5-year asset smoothing, DR 6.4%, ir 7.12%, sd 12%; Preset MA</t>
+  </si>
+  <si>
+    <t>6.62% / 12%</t>
+  </si>
+  <si>
+    <t>7.12% / 12%</t>
+  </si>
+  <si>
+    <t>geo-mean implied by DR 6.4%</t>
+  </si>
+  <si>
+    <t>DR based on lower treasury rate</t>
+  </si>
+  <si>
+    <t>DR based on lower treasury rate; geo-mean implied by DR 5.9%</t>
+  </si>
+  <si>
+    <t>100% initial Funding; DC 7.5; ir 4.5,    SD 4.5%</t>
+  </si>
+  <si>
+    <t>100% initial Funding; DC 7.5; ir 6,        SD 8.3%</t>
+  </si>
+  <si>
+    <t>100% initial Funding; DC 7.5; ir 7.5,    SD 12%</t>
+  </si>
+  <si>
+    <t>100% initial Funding; DC 7.5; ir 9,        SD 15.8%</t>
+  </si>
+  <si>
+    <t>100% initial Funding; DC 7.5; ir 10.5,  SD 19.5%</t>
   </si>
 </sst>
 </file>
@@ -1350,7 +1362,7 @@
     <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyBorder="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyBorder="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="41">
+  <cellXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1430,6 +1442,9 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -1532,14 +1547,14 @@
       <sheetName val="Sheet1"/>
     </sheetNames>
     <sheetDataSet>
-      <sheetData sheetId="0"/>
-      <sheetData sheetId="1"/>
-      <sheetData sheetId="2"/>
-      <sheetData sheetId="3"/>
-      <sheetData sheetId="4"/>
-      <sheetData sheetId="5"/>
+      <sheetData sheetId="0" refreshError="1"/>
+      <sheetData sheetId="1" refreshError="1"/>
+      <sheetData sheetId="2" refreshError="1"/>
+      <sheetData sheetId="3" refreshError="1"/>
+      <sheetData sheetId="4" refreshError="1"/>
+      <sheetData sheetId="5" refreshError="1"/>
       <sheetData sheetId="6"/>
-      <sheetData sheetId="7"/>
+      <sheetData sheetId="7" refreshError="1"/>
     </sheetDataSet>
   </externalBook>
 </externalLink>
@@ -11993,10 +12008,10 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AR37"/>
+  <dimension ref="A1:AR40"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="E28" sqref="E28"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -12006,11 +12021,12 @@
     <col min="3" max="3" width="110" customWidth="1"/>
     <col min="4" max="4" width="13.140625" customWidth="1"/>
     <col min="5" max="5" width="18.5703125" customWidth="1"/>
+    <col min="6" max="6" width="58" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="35" t="s">
-        <v>376</v>
+        <v>370</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
@@ -12120,7 +12136,7 @@
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="39" t="s">
-        <v>370</v>
+        <v>364</v>
       </c>
       <c r="B11" s="38" t="s">
         <v>304</v>
@@ -12200,7 +12216,7 @@
         <v>324</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" s="39"/>
       <c r="B17" t="s">
         <v>300</v>
@@ -12215,7 +12231,7 @@
         <v>324</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" s="39"/>
       <c r="B18" t="s">
         <v>301</v>
@@ -12230,9 +12246,9 @@
         <v>324</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" s="39" t="s">
-        <v>370</v>
+        <v>364</v>
       </c>
       <c r="B19" s="38" t="s">
         <v>302</v>
@@ -12247,7 +12263,7 @@
         <v>324</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" s="39"/>
       <c r="B20" t="s">
         <v>303</v>
@@ -12262,13 +12278,13 @@
         <v>324</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" s="39"/>
       <c r="B21" s="37" t="s">
-        <v>371</v>
+        <v>365</v>
       </c>
       <c r="C21" s="22" t="s">
-        <v>372</v>
+        <v>366</v>
       </c>
       <c r="D21" s="27">
         <v>7.4999999999999997E-2</v>
@@ -12277,7 +12293,7 @@
         <v>324</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" s="39"/>
       <c r="B22" t="s">
         <v>307</v>
@@ -12287,18 +12303,13 @@
       </c>
       <c r="D22" s="27"/>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" s="39"/>
-      <c r="D23" s="27">
-        <v>7.4999999999999997E-2</v>
-      </c>
-      <c r="E23" t="s">
-        <v>324</v>
-      </c>
+      <c r="D23" s="27"/>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" s="39" t="s">
-        <v>370</v>
+        <v>364</v>
       </c>
       <c r="B24" s="38" t="s">
         <v>317</v>
@@ -12313,28 +12324,30 @@
         <v>324</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25" s="39"/>
       <c r="B25" t="s">
         <v>318</v>
       </c>
       <c r="C25" s="22" t="s">
-        <v>368</v>
+        <v>373</v>
       </c>
       <c r="D25" s="27">
         <v>6.4000000000000001E-2</v>
       </c>
       <c r="E25" t="s">
-        <v>369</v>
+        <v>375</v>
+      </c>
+      <c r="F25" t="s">
+        <v>376</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A26" s="39"/>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B26" s="40" t="s">
         <v>319</v>
       </c>
       <c r="C26" s="22" t="s">
-        <v>377</v>
+        <v>371</v>
       </c>
       <c r="D26" s="27">
         <v>5.8999999999999997E-2</v>
@@ -12342,27 +12355,32 @@
       <c r="E26" t="s">
         <v>324</v>
       </c>
+      <c r="F26" s="41" t="s">
+        <v>377</v>
+      </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A27" s="39"/>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B27" t="s">
-        <v>367</v>
+        <v>363</v>
       </c>
       <c r="C27" s="22" t="s">
-        <v>378</v>
+        <v>372</v>
       </c>
       <c r="D27" s="27">
         <v>5.8999999999999997E-2</v>
       </c>
       <c r="E27" t="s">
-        <v>379</v>
+        <v>374</v>
+      </c>
+      <c r="F27" s="41" t="s">
+        <v>378</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="C28" s="22"/>
       <c r="D28" s="27"/>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A29" s="36" t="s">
         <v>291</v>
       </c>
@@ -12373,7 +12391,7 @@
         <v>324</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B30" t="s">
         <v>323</v>
       </c>
@@ -12387,7 +12405,7 @@
         <v>324</v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B31" s="37" t="s">
         <v>320</v>
       </c>
@@ -12401,7 +12419,7 @@
         <v>324</v>
       </c>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B32" s="37" t="s">
         <v>321</v>
       </c>
@@ -12453,7 +12471,7 @@
         <v>218</v>
       </c>
       <c r="C36" s="22" t="s">
-        <v>373</v>
+        <v>367</v>
       </c>
       <c r="D36" s="27">
         <v>7.4999999999999997E-2</v>
@@ -12486,13 +12504,13 @@
     </row>
     <row r="37" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A37" s="39" t="s">
-        <v>375</v>
+        <v>369</v>
       </c>
       <c r="B37" s="37" t="s">
         <v>219</v>
       </c>
       <c r="C37" s="22" t="s">
-        <v>374</v>
+        <v>368</v>
       </c>
       <c r="D37" s="27">
         <v>7.4999999999999997E-2</v>
@@ -12522,6 +12540,12 @@
       <c r="AP37" s="21"/>
       <c r="AQ37" s="21"/>
       <c r="AR37" s="21"/>
+    </row>
+    <row r="40" spans="1:44" x14ac:dyDescent="0.25">
+      <c r="C40">
+        <f>0.12^2/2 + 0.059</f>
+        <v>6.6199999999999995E-2</v>
+      </c>
     </row>
   </sheetData>
   <dataValidations disablePrompts="1" count="20">
@@ -12629,7 +12653,7 @@
   <dimension ref="A1:XFD35"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B32" sqref="B32"/>
+      <selection activeCell="C30" sqref="C30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -12643,7 +12667,7 @@
   <sheetData>
     <row r="1" spans="1:16384" x14ac:dyDescent="0.25">
       <c r="A1" s="35" t="s">
-        <v>376</v>
+        <v>370</v>
       </c>
       <c r="B1" s="35"/>
       <c r="C1" s="35"/>
@@ -45504,6 +45528,9 @@
       <c r="C11" s="22" t="s">
         <v>349</v>
       </c>
+      <c r="D11" s="27" t="s">
+        <v>109</v>
+      </c>
     </row>
     <row r="12" spans="1:16384" x14ac:dyDescent="0.25">
       <c r="A12" s="35"/>
@@ -45513,6 +45540,9 @@
       <c r="C12" s="22" t="s">
         <v>351</v>
       </c>
+      <c r="D12" s="27" t="s">
+        <v>109</v>
+      </c>
     </row>
     <row r="13" spans="1:16384" x14ac:dyDescent="0.25">
       <c r="A13" s="35"/>
@@ -45522,6 +45552,9 @@
       <c r="C13" s="22" t="s">
         <v>353</v>
       </c>
+      <c r="D13" s="27" t="s">
+        <v>109</v>
+      </c>
     </row>
     <row r="14" spans="1:16384" x14ac:dyDescent="0.25">
       <c r="B14" s="37" t="s">
@@ -45530,6 +45563,9 @@
       <c r="C14" s="22" t="s">
         <v>355</v>
       </c>
+      <c r="D14" s="27" t="s">
+        <v>109</v>
+      </c>
     </row>
     <row r="15" spans="1:16384" x14ac:dyDescent="0.25">
       <c r="B15" s="37" t="s">
@@ -45538,83 +45574,110 @@
       <c r="C15" s="22" t="s">
         <v>357</v>
       </c>
+      <c r="D15" s="27" t="s">
+        <v>109</v>
+      </c>
     </row>
     <row r="16" spans="1:16384" x14ac:dyDescent="0.25">
       <c r="C16" s="22"/>
+      <c r="D16" s="27"/>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B17" t="s">
         <v>358</v>
       </c>
       <c r="C17" s="22" t="s">
+        <v>379</v>
+      </c>
+      <c r="D17" s="27" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B18" t="s">
         <v>359</v>
       </c>
+      <c r="C18" s="22" t="s">
+        <v>380</v>
+      </c>
+      <c r="D18" s="27" t="s">
+        <v>109</v>
+      </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B18" t="s">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B19" t="s">
         <v>360</v>
       </c>
-      <c r="C18" s="22" t="s">
+      <c r="C19" s="22" t="s">
+        <v>381</v>
+      </c>
+      <c r="D19" s="27" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B20" t="s">
         <v>361</v>
       </c>
+      <c r="C20" s="22" t="s">
+        <v>382</v>
+      </c>
+      <c r="D20" s="27" t="s">
+        <v>109</v>
+      </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B19" t="s">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B21" t="s">
         <v>362</v>
       </c>
-      <c r="C19" s="22" t="s">
-        <v>353</v>
+      <c r="C21" s="22" t="s">
+        <v>383</v>
+      </c>
+      <c r="D21" s="27" t="s">
+        <v>109</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B20" t="s">
-        <v>363</v>
-      </c>
-      <c r="C20" s="22" t="s">
-        <v>364</v>
-      </c>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C22" s="22"/>
+      <c r="D22" s="27"/>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B21" t="s">
-        <v>365</v>
-      </c>
-      <c r="C21" s="22" t="s">
-        <v>366</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="C22" s="22"/>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" s="35" t="s">
         <v>346</v>
       </c>
+      <c r="D23" s="27"/>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B24" s="37" t="s">
         <v>342</v>
       </c>
       <c r="C24" s="22" t="s">
         <v>343</v>
       </c>
+      <c r="D24" s="27" t="s">
+        <v>109</v>
+      </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B25" s="37" t="s">
         <v>344</v>
       </c>
       <c r="C25" s="22" t="s">
         <v>345</v>
       </c>
+      <c r="D25" s="27" t="s">
+        <v>109</v>
+      </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" s="35" t="s">
         <v>347</v>
       </c>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C31" s="22"/>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C32" s="22"/>
     </row>
     <row r="33" spans="3:3" x14ac:dyDescent="0.25">

</xml_diff>